<commit_message>
EXCEL file w/copar weight.avg. values for diff techs. (ONight & OM)
</commit_message>
<xml_diff>
--- a/Generation/costo_unitario_de_inversion.xlsx
+++ b/Generation/costo_unitario_de_inversion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="2400" windowWidth="18720" windowHeight="20040" tabRatio="991"/>
+    <workbookView xWindow="10300" yWindow="460" windowWidth="16440" windowHeight="19300" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="lola" sheetId="1" r:id="rId1"/>
@@ -434,11 +434,12 @@
   <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="5"/>
     <col min="10" max="10" width="8.83203125" style="2"/>
   </cols>

</xml_diff>